<commit_message>
Integrated and tested institutions normalization after concatenation and deduplication of corpuses parsing
</commit_message>
<xml_diff>
--- a/BiblioParsing/BiblioParsing_RefFiles/Inst_types.xlsx
+++ b/BiblioParsing/BiblioParsing_RefFiles/Inst_types.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amal/My_Jupyter/BiblioAnalysis/BiblioAnalysis_Utils/BiblioAnalysis_RefFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC265100\PyVenv\BiblioParsing\BiblioParsing\BiblioParsing_RefFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED17938B-BBCA-E542-BCF5-08993211092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38480" yWindow="-1540" windowWidth="31820" windowHeight="23320" xr2:uid="{0BAB19F8-7608-514D-95BB-6D34C93C1D02}"/>
+    <workbookView xWindow="-38475" yWindow="-1545" windowWidth="31815" windowHeight="23325"/>
   </bookViews>
   <sheets>
     <sheet name="Norm affiliation types" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
   <si>
     <t>Agn</t>
   </si>
@@ -285,12 +284,18 @@
   </si>
   <si>
     <t>Lab</t>
+  </si>
+  <si>
+    <t>Labex</t>
+  </si>
+  <si>
+    <t>Laboratoire d'excellence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -655,23 +660,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F44B919-1814-704F-947D-6CD4E9EAC661}">
-  <dimension ref="A1:D30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="1"/>
+    <col min="5" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -685,7 +690,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -699,7 +704,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -713,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -727,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -741,7 +746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -755,7 +760,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -769,7 +774,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -783,7 +788,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -797,7 +802,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -811,7 +816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -825,7 +830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -839,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -853,7 +858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -867,7 +872,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -881,7 +886,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -895,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -909,7 +914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -923,7 +928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -937,7 +942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -951,7 +956,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -965,7 +970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -979,7 +984,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -993,7 +998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1021,78 +1026,92 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:D44">
+  <sortState ref="B10:D44">
     <sortCondition ref="B1:B44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>